<commit_message>
Added Mockup Task, because it's almost done
</commit_message>
<xml_diff>
--- a/doc/taskOverview/tasks.xlsx
+++ b/doc/taskOverview/tasks.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ti4ac12\Documents\TAE_ProjectManagement\doc\taskOverview\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="120" yWindow="105" windowWidth="28515" windowHeight="12600"/>
   </bookViews>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>PCM Tasks (name tbd)</t>
   </si>
@@ -152,14 +157,17 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
-    <a:clrScheme name="Larissa">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -197,9 +205,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Larissa">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -234,7 +242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -269,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Larissa">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -531,6 +539,9 @@
       <c r="A13" t="s">
         <v>8</v>
       </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">

</xml_diff>